<commit_message>
Added Webscraping for Webhallen
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -455,7 +455,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.webhallen.com/se/product/232445-Logitech-C920-HD-Pro-Webcam</t>
+          <t>https://www.webhallen.com/api/product/232445</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -499,7 +499,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1190.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>